<commit_message>
Update .gitignore and untrack unnecessary files
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shana\source\repos\NUnitSeleniumTraining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB2C33C-E23F-46FE-AED4-E8AFD7928635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E639DE50-B1DD-49F6-BCE6-04A6144871BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,16 +39,16 @@
     <t>xygygux</t>
   </si>
   <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>admin@gmail.com</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>asdfgfsg</t>
+  </si>
+  <si>
+    <t>ssfsfs</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -391,10 +391,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -415,17 +415,17 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{6AAFA724-4ADD-4125-B745-82E98301FDD8}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{E96BE051-B84F-44ED-965E-AC3CC6E90E18}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{E85A9794-D842-41F6-9DD0-4A656A48AD30}"/>
+    <hyperlink ref="A4" r:id="rId3" display="admin@gmail.com" xr:uid="{E85A9794-D842-41F6-9DD0-4A656A48AD30}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>